<commit_message>
New changes test cases
</commit_message>
<xml_diff>
--- a/POMExample/uiAutomation/src/main/java/com/test/automation/uiAutomation/data/LoginTestData.xlsx
+++ b/POMExample/uiAutomation/src/main/java/com/test/automation/uiAutomation/data/LoginTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6225"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -27,35 +27,26 @@
     <t>runMode</t>
   </si>
   <si>
-    <t>test</t>
+    <t>authenticated-user-test@mailinator.com</t>
+  </si>
+  <si>
+    <t>authenticatedusertest</t>
   </si>
   <si>
     <t>y</t>
   </si>
   <si>
-    <t>p@mail.com</t>
-  </si>
-  <si>
-    <t>p@test.com</t>
-  </si>
-  <si>
-    <t>per@maill.com</t>
-  </si>
-  <si>
-    <t>Pst@mail.com</t>
-  </si>
-  <si>
-    <t>pd@mail.com</t>
-  </si>
-  <si>
-    <t>ps@mail.com</t>
+    <t>pratik.sidam@cactusglobal.com</t>
+  </si>
+  <si>
+    <t>pratik.sidam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +61,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,9 +90,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,106 +403,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:authenticated-user-test@mailinator.com"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>